<commit_message>
refined node and developer states and incorporated logic into function
</commit_message>
<xml_diff>
--- a/Thesis/developer_states.xlsx
+++ b/Thesis/developer_states.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="214" documentId="8_{A4B64DE1-C1F9-4DF8-A805-E80C52345F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{649E1524-1684-45AB-AC93-495F54A48BA6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{31558D2F-F994-4500-BC80-1C41F5323AB0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{31558D2F-F994-4500-BC80-1C41F5323AB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1815,8 +1815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB29B94B-9539-40D3-B7DF-08904E974596}">
   <dimension ref="A1:G315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A300" workbookViewId="0">
-      <selection activeCell="H314" sqref="H314"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>